<commit_message>
Update for MathNet.Numerics library
</commit_message>
<xml_diff>
--- a/CAPI-Licences.xlsx
+++ b/CAPI-Licences.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehdi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pat\source\repos\CAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF0F63F-BD4D-4EC3-BE39-A02DE5A7DFCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="13860"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>ClearCanvas</t>
   </si>
@@ -108,12 +109,21 @@
   </si>
   <si>
     <t>https://www.nitrc.org/projects/cmtk</t>
+  </si>
+  <si>
+    <t>MathNet.Numerics</t>
+  </si>
+  <si>
+    <t>MIT/X11</t>
+  </si>
+  <si>
+    <t>https://numerics.mathdotnet.com/License.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,15 +192,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -471,10 +493,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -614,6 +638,17 @@
       </c>
       <c r="E9" s="2"/>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pre-merge (already in master)
</commit_message>
<xml_diff>
--- a/CAPI-Licences.xlsx
+++ b/CAPI-Licences.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mehdi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pat\source\repos\CAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF0F63F-BD4D-4EC3-BE39-A02DE5A7DFCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="13860"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>ClearCanvas</t>
   </si>
@@ -108,12 +109,21 @@
   </si>
   <si>
     <t>https://www.nitrc.org/projects/cmtk</t>
+  </si>
+  <si>
+    <t>MathNet.Numerics</t>
+  </si>
+  <si>
+    <t>MIT/X11</t>
+  </si>
+  <si>
+    <t>https://numerics.mathdotnet.com/License.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,15 +192,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -471,10 +493,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -614,6 +638,17 @@
       </c>
       <c r="E9" s="2"/>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added license for CSS.
</commit_message>
<xml_diff>
--- a/CAPI-Licences.xlsx
+++ b/CAPI-Licences.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pat\source\repos\CAPI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF0F63F-BD4D-4EC3-BE39-A02DE5A7DFCB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>ClearCanvas</t>
   </si>
@@ -54,9 +48,6 @@
     <t>https://clearcanvas.github.io/</t>
   </si>
   <si>
-    <t>GNU</t>
-  </si>
-  <si>
     <t>http://brainsuite.org/</t>
   </si>
   <si>
@@ -118,13 +109,28 @@
   </si>
   <si>
     <t>https://numerics.mathdotnet.com/License.html</t>
+  </si>
+  <si>
+    <t>https://www.creative-tim.com/product/now-ui-dashboard</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>Now UI Dashboard</t>
+  </si>
+  <si>
+    <t>WebService/assets</t>
+  </si>
+  <si>
+    <t>CSS template for web service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +142,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -204,18 +218,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,18 +506,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,19 +531,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -532,9 +552,9 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="2"/>
@@ -547,13 +567,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -564,10 +584,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -579,10 +599,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -594,10 +614,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -606,51 +626,72 @@
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="E11" s="6" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>